<commit_message>
made graph, checked outliers, ready for analysis on Tuesday
</commit_message>
<xml_diff>
--- a/Resources/Deforestation.xlsx
+++ b/Resources/Deforestation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spyro\Documents\UWA Boot Camp\Projects\Disney Donut\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spyro\Documents\UWA Boot Camp\Projects\disney-donut-project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B9C1C5-F631-4939-A787-7CD28B4EAC14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9366E202-6C53-4418-87BC-390A192EE4AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2B9900B-1E04-4926-8E17-608D7CDAA5F4}"/>
   </bookViews>
@@ -87,7 +87,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -100,7 +100,6 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F553D0-0DF4-4722-BB19-F35C9DBB2C59}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +425,7 @@
     <col min="1" max="2" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,227 +433,358 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="B2" s="4">
-        <v>133.88215206367161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133.68096809673614</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="B3" s="4">
-        <v>133.68096809673614</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133.44748662356463</v>
+      </c>
+      <c r="C3">
+        <f>B3/B2-1</f>
+        <v>-1.7465573184849426E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="B4" s="4">
-        <v>133.44748662356463</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133.24491623764933</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C27" si="0">B4/B3-1</f>
+        <v>-1.5179782777529072E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="B5" s="4">
-        <v>133.24491623764933</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132.98286057652842</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-1.9667216470271587E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="B6" s="4">
-        <v>132.98286057652842</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132.8769677231607</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>-7.9628948353671625E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="B7" s="4">
-        <v>132.8769677231607</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132.73626401072818</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-1.0589021923322894E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="B8" s="4">
-        <v>132.73626401072818</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132.56742008097785</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-1.2720256292333421E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="B9" s="4">
-        <v>132.56742008097785</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132.37300679797053</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>-1.4665238479301124E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="B10" s="4">
-        <v>132.37300679797053</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132.1216174894335</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>-1.8990979703339406E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="B11" s="4">
-        <v>132.1216174894335</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131.81410232161582</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>-2.3275159179932947E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="B12" s="4">
-        <v>131.81410232161582</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131.35787266824858</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>-3.4611596584261939E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B13" s="4">
-        <v>131.35787266824858</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130.95274470674352</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>-3.084154404115802E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B14" s="4">
-        <v>130.95274470674352</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130.60433741668731</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>-2.660557370037786E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B15" s="4">
-        <v>130.60433741668731</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130.26282055788673</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-2.614896760365526E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B16" s="4">
-        <v>130.26282055788673</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129.75006825689675</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>-3.9362904840688495E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="B17" s="4">
-        <v>129.75006825689675</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129.29919495903857</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>-3.4749368837747596E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B18" s="4">
-        <v>129.29919495903857</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>128.9740678033387</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>-2.5145334880304349E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B19" s="4">
-        <v>128.9740678033387</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>128.94060010426247</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>-2.5949169198302702E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B20" s="4">
-        <v>128.94060010426247</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129.14751378734633</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>1.6047209561342868E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B21" s="4">
-        <v>129.14751378734633</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>129.5461099836964</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>3.086363683364457E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B22" s="4">
-        <v>129.5461099836964</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130.12449435099097</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>4.4646988424998924E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B23" s="4">
-        <v>130.12449435099097</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>130.76072823016156</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>4.8894244111676866E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B24" s="4">
-        <v>130.76072823016156</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131.41342538388295</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>4.9915380753502436E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B25" s="4">
-        <v>131.41342538388295</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>132.21450974136854</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>6.0959095704680166E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B26" s="4">
-        <v>132.21450974136854</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>133.09449343053021</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>6.6557270520690714E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>2015</v>
-      </c>
-      <c r="B27" s="4">
-        <v>133.09449343053021</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2016</v>
+      </c>
+      <c r="B27" s="5">
+        <v>134.04</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>7.104024705299361E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>2016</v>
-      </c>
-      <c r="B28" s="5">
-        <v>134.04</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
+        <v>2017</v>
+      </c>
+      <c r="B28" s="4">
+        <f>B27*(AVERAGE($C$20:$C$27))+B27</f>
+        <v>134.69164228425038</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" ref="B29:B31" si="1">B28*(AVERAGE($C$20:$C$27))+B28</f>
+        <v>135.34645256064209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" si="1"/>
+        <v>136.00444623053022</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" si="1"/>
+        <v>136.66563877014431</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>